<commit_message>
Update to CTF v1.5 open source release
</commit_message>
<xml_diff>
--- a/docs/masters/CTF_Test_Instruction_Reference.xlsx
+++ b/docs/masters/CTF_Test_Instruction_Reference.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twchrist\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D2FB1CF-DCA1-4284-9BE5-15AA94470F12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B040EA60-4B13-463C-B2DB-5EE7E42A01D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5595" windowWidth="38640" windowHeight="21840" xr2:uid="{D1E9E584-E375-4391-A0A9-95834F0EFA31}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1E9E584-E375-4391-A0A9-95834F0EFA31}"/>
   </bookViews>
   <sheets>
     <sheet name="Open Source" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Open Source'!$B$2:$F$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Open Source'!$B$2:$F$44</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Open Source'!$4:$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="166">
   <si>
     <t>CTF Instructions</t>
   </si>
@@ -682,20 +682,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">target:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>name of a registered cFS target; i.e. executable cFS image</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <i/>
@@ -748,41 +734,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">target:  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">name of a registered cFS target; i.e. executable cFS image
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>run_args:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  command line argument for cFS executable</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <i/>
@@ -1004,39 +955,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>verification_id:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  the verification_id value of an existing </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>CheckTlmContinuous</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t>target:</t>
     </r>
     <r>
@@ -1102,6 +1020,27 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
+      <t>host:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  network hostname or IP to connect to
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
       <t>name:</t>
     </r>
     <r>
@@ -1111,49 +1050,6 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">  an arbitrary-but-unique name to identified an SSH target</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>host:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  network hostname or IP to connect to
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
       <t xml:space="preserve">  a registered SSH target; optional
 </t>
     </r>
@@ -1300,49 +1196,6 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve">  additional SSH connection options, as needed</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  a registered SSH target
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>command:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  the shell command to be executed; can contain multiple commands separated with semicolon</t>
     </r>
   </si>
   <si>
@@ -2128,112 +1981,6 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve">  value of primitive data type (e.g., integer, float or string)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>label:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  user-define label; must be unique within the scope of the test case
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>conditions:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  a list of comparison conditions
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>condition.name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  name of an existing user-defined variable
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>condition.operator:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  comparison operator
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>condition.value:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  value of primitive data type</t>
     </r>
   </si>
   <si>
@@ -2298,192 +2045,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>target:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  name of a registered cFS target; optional; default is empty string; if not specified, it applies to </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>all</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> registered cFS targets
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>app_name:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  the name of the cFS application that sent the event message
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>event_id:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  cFS event ID
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>event_str:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  the event message; optional; default is empty string; if specified, CTF performs a string comparison between the expected and actual strings
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>is_regex:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  boolean flag to denote a regex match instead of string comparison is to be performed on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>event_str</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">; optional; default is false
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>event_str_args:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">  arguments that will be inserted into </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>event_str</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>, similar to printf() function; optional; default is empty string</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Have CTF verify that one or more cFS events matching the specified parameters </t>
     </r>
     <r>
@@ -2874,6 +2435,1056 @@
         "hex_buffer": "0123456789ABCDEF"
    }
 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IfCondition</t>
+  </si>
+  <si>
+    <t>ElseCondition</t>
+  </si>
+  <si>
+    <t>EndCondition</t>
+  </si>
+  <si>
+    <t>Have CTF create a ifcondition exit point and associate it with the specified label</t>
+  </si>
+  <si>
+    <t>{
+    "instruction":  "EndCondition",
+    "data": {
+        "label": "If_Label_1"
+    }
+}</t>
+  </si>
+  <si>
+    <t>{
+    "instruction":  "ElseCondition",
+    "data": {
+        "label": "If_Label_1"
+    }
+}</t>
+  </si>
+  <si>
+    <t>Have CTF create an entry point for else conditional branch block and associate it with the specified label. If the condition of IfCondition instruction is False, the control flow skips the 'if' branch block, and executes the 'else' branch block</t>
+  </si>
+  <si>
+    <t>{
+    "instruction":  "IfCondition",
+    "data": {
+        "label": "If_Label_1",
+        "conditions": [
+            { "variable": "my_var_1",  
+              "compare":  "&lt;",
+              "value": 4
+            },
+            { "variable": "my_var_2",
+              "compare": "&gt;",
+              "value": 1
+            }
+        ]
+    }
+}</t>
+  </si>
+  <si>
+    <t>Have CTF create a conditional branch entry point and associate it with the specified label; commonly use to execute or skip a set of test instructions based on comparision results.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validation </t>
+  </si>
+  <si>
+    <t>CopyFiles</t>
+  </si>
+  <si>
+    <t>DeleteFiles</t>
+  </si>
+  <si>
+    <t>SearchStr</t>
+  </si>
+  <si>
+    <t>SaveFileAsText</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>source:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  path of the file / folder to be copied from on host machine
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>destination:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  path of the file / folder to be copied to on host machine</t>
+    </r>
+  </si>
+  <si>
+    <t>Copy a file or folder on the host file system. If the destination exists, it will be overridden.</t>
+  </si>
+  <si>
+    <t>{
+    "instruction":  "CopyFiles",
+    "data": {
+        "source": "./testArtifacts1",
+        "destination": "./testArtifacts2"
+    }
+}</t>
+  </si>
+  <si>
+    <t>Delete a file or folder on the host file system.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>path:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  path of the file / folder to be deleted on host machine.</t>
+    </r>
+  </si>
+  <si>
+    <t>{
+    "instruction":  "DeleteFiles",
+    "data": {
+        "path": "./testArtifacts1"        
+    }
+}</t>
+  </si>
+  <si>
+    <t>Search a text file for a given text string.</t>
+  </si>
+  <si>
+    <t>{
+    "instruction":  "SearchStr",
+    "data": {
+        "file": "/testArtifacts/event_log.txt",
+        "search_str": "computer reboot"
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>file:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  path of the text file
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>search_str:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  text string to search</t>
+    </r>
+  </si>
+  <si>
+    <t>Save the cFE event log file (binary file created via the CFE_EVS_WRITE_LOG_DATA_FILE_CC command) to a human-readable text file</t>
+  </si>
+  <si>
+    <t>{
+    "instruction":  "SaveFileAsText",
+    "data": {
+        "input_file": "/dev/shm/osal:RAM/event.bin",
+        "output_file": "./testArtifacts/event_log.txt",
+        "file_type": "EVS",
+        "target": "cfs"
+    }
+}</t>
+  </si>
+  <si>
+    <t>SetUserVariableFromTlmHeader</t>
+  </si>
+  <si>
+    <t>Have CTF create a variable and assign a value of a telemetry header field to it</t>
+  </si>
+  <si>
+    <t>{
+    "instruction":  "SetUserVariableFromTlmHeader",
+    "data": {
+        "variable_name": "my_var_2",
+        "mid": "TO_HL_TLM_MID",
+        "header_variable": "pheader.length"
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t>target:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  name of a registered cFS target; optional; default is empty string; if not specified, it applies to all registered cFS targets
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>run_args:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  command line argument for cFS executable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>target:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  name of a registered cFS target; optional; default is empty string; if not specified, it applies to all registered cFS targets</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>target:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  name of a registered cFS target; optional; default is empty string; if not specified, it applies to </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> registered cFS targets
+args:  a list of objects with the following:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    app_name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  the name of the cFS application that sent the event message
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    event_id:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  cFS event ID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    event_str:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  the event message; optional; default is empty string; if specified, CTF performs a string comparison between the expected and actual strings
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    is_regex:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  boolean flag to denote a regex match instead of string comparison is to be performed on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>event_str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">; optional; default is false
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    event_str_args:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  arguments that will be inserted into </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>event_str</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, similar to printf() function; optional; default is empty string</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>target:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  name of a registered cFS target; optional; default is empty string; if not specified, it applies to all registered cFS targets</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+verification_id:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  the verification_id value of an existing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>CheckTlmContinuous</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  an arbitrary-but-unique name to identify an SSH target</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>name:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  a registered SSH target
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>command:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  the shell command to be executed; can contain multiple commands separated with semicolon
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>cwd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: current working directory in which to execute command; optional
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>prefix</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: an additional command to execute before command whose result is ignored; optional</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>variable_name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  user-defined variable name
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>mid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  CCSDS message ID
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>header_variable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:  name of the telemetry item as defined in the json definition for CCSDS headers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>input_file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  path of the binary event log file
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>output_file</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  path of the output text file.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>file_type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">: currently only supports 'EVS' file type
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>target</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>: cfs target, optional</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  user-defined label; must match an existing label from </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>IfCondition</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> instruction</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>label:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  user-defined label; must be unique within the scope of the test case
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>conditions:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  a list of comparison conditions
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>condition.variable:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  name of an existing user-defined variable
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>condition.compare:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  comparison operator
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>condition.value:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  value of primitive data type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>label</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  user-defined label; must be unique within the scope of the test case
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>conditions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  a list of comparison conditions
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>condition.variable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  name of an existing user-defined variable
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>condition.compare</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">:  comparison operator
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>condition.value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>:  value of primitive data type</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2943,7 +3554,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -3072,14 +3683,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3119,9 +3738,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -3140,7 +3756,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3172,10 +3787,40 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3497,589 +4142,725 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13207C2A-CCFD-4D3B-B0C4-FC7E315016DA}">
-  <dimension ref="A2:K37"/>
+  <dimension ref="A2:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33.5703125" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" style="18" customWidth="1"/>
-    <col min="5" max="5" width="47" style="15" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="47" style="14" customWidth="1"/>
     <col min="6" max="6" width="50.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:6" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:6" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+    <row r="5" spans="1:6" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="D5" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="28" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="24" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E7" s="7" t="s">
+      <c r="D7" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8" s="22" t="s">
+      <c r="D8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="30" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:6" ht="248.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="7" t="s">
+      <c r="D9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="24" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21"/>
+      <c r="B11" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>129</v>
-      </c>
     </row>
-    <row r="11" spans="1:6" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="32" t="s">
+    <row r="12" spans="1:6" ht="282.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" s="36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="258.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>123</v>
+      <c r="D12" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="187.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="F13" s="27" t="s">
-        <v>124</v>
+      <c r="E13" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="165" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E14" s="7" t="s">
+      <c r="D14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="24" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E15" s="7" t="s">
+      <c r="D15" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="24" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E16" s="7" t="s">
+      <c r="D16" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="24" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="17" spans="2:11" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="D17" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="K17" s="34"/>
+      <c r="K17" s="31"/>
     </row>
-    <row r="18" spans="2:11" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="2:11" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" s="14" t="s">
+      <c r="D18" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="24" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:11" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="D19" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="27" t="s">
+      <c r="F19" s="24" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" s="22" t="s">
+      <c r="D20" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E21" s="7" t="s">
+      <c r="D21" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="27" t="s">
+      <c r="F21" s="24" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="195.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="2:11" ht="215.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" s="7" t="s">
+      <c r="D22" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="24" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="2:11" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="7" t="s">
+      <c r="D23" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="24" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:11" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="E24" s="7" t="s">
+      <c r="D24" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="27" t="s">
+      <c r="F24" s="24" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="25" spans="2:11" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" s="7" t="s">
+      <c r="D25" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="27" t="s">
+      <c r="F25" s="24" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="26" spans="2:11" ht="211.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E26" s="7" t="s">
+      <c r="D26" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="27" t="s">
+      <c r="F26" s="24" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="27" spans="2:11" ht="212.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E27" s="7" t="s">
+      <c r="D27" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F27" s="27" t="s">
+      <c r="F27" s="24" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="28" spans="2:11" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="E28" s="7" t="s">
+      <c r="D28" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F28" s="27" t="s">
+      <c r="F28" s="24" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="29" spans="2:11" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E29" s="7" t="s">
+      <c r="D29" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="27" t="s">
+      <c r="F29" s="24" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="30" spans="2:11" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="7" t="s">
+      <c r="D30" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="27" t="s">
+      <c r="F30" s="24" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="31" spans="2:11" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E31" s="7" t="s">
+      <c r="D31" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F31" s="27" t="s">
+      <c r="F31" s="24" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="32" spans="2:11" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E32" s="7" t="s">
+      <c r="D32" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="27" t="s">
+      <c r="F32" s="24" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+    <row r="33" spans="2:6" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="E33" s="7" t="s">
+      <c r="D34" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="27" t="s">
+      <c r="F34" s="24" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="189" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="28" t="s">
+    <row r="35" spans="2:6" ht="189" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C35" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D34" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="22" t="s">
+      <c r="D35" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F34" s="27" t="s">
-        <v>119</v>
+      <c r="F35" s="24" t="s">
+        <v>113</v>
       </c>
     </row>
-    <row r="35" spans="2:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+    <row r="36" spans="2:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" s="7" t="s">
+      <c r="D36" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F35" s="27" t="s">
+      <c r="F36" s="24" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="5"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="23"/>
+    <row r="37" spans="2:6" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="37" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C37" s="1"/>
-      <c r="D37" s="21"/>
-      <c r="E37" s="17"/>
+    <row r="38" spans="2:6" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F38" s="33" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" s="36" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F40" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="F42" s="33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="109.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E43" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="F43" s="45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="38"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="42"/>
+    </row>
+    <row r="45" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C45" s="1"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>